<commit_message>
chore: Prevent writing new useful_checks.xlsx if it is already up to date
</commit_message>
<xml_diff>
--- a/income_sheet.xlsx
+++ b/income_sheet.xlsx
@@ -1191,7 +1191,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E216"/>
+  <dimension ref="A1:E220"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -5092,6 +5092,78 @@
         <v>386</v>
       </c>
     </row>
+    <row r="217" ht="13.55" customHeight="1">
+      <c r="A217" s="3">
+        <v>44905</v>
+      </c>
+      <c r="B217" s="4">
+        <v>166</v>
+      </c>
+      <c r="C217" s="4">
+        <v>6.5</v>
+      </c>
+      <c r="D217" s="4">
+        <v>15</v>
+      </c>
+      <c r="E217" s="4">
+        <f>B217+(C217*D217)</f>
+        <v>263.5</v>
+      </c>
+    </row>
+    <row r="218" ht="13.55" customHeight="1">
+      <c r="A218" s="3">
+        <v>44906</v>
+      </c>
+      <c r="B218" s="4">
+        <v>257</v>
+      </c>
+      <c r="C218" s="4">
+        <v>6.5</v>
+      </c>
+      <c r="D218" s="4">
+        <v>15</v>
+      </c>
+      <c r="E218" s="4">
+        <f>B218+(C218*D218)</f>
+        <v>354.5</v>
+      </c>
+    </row>
+    <row r="219" ht="13.55" customHeight="1">
+      <c r="A219" s="3">
+        <v>44908</v>
+      </c>
+      <c r="B219" s="4">
+        <v>45</v>
+      </c>
+      <c r="C219" s="4">
+        <v>4</v>
+      </c>
+      <c r="D219" s="4">
+        <v>15</v>
+      </c>
+      <c r="E219" s="4">
+        <f>B219+(C219*D219)</f>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="220" ht="13.55" customHeight="1">
+      <c r="A220" s="3">
+        <v>44909</v>
+      </c>
+      <c r="B220" s="4">
+        <v>155</v>
+      </c>
+      <c r="C220" s="4">
+        <v>6.5</v>
+      </c>
+      <c r="D220" s="4">
+        <v>15</v>
+      </c>
+      <c r="E220" s="4">
+        <f>B220+(C220*D220)</f>
+        <v>252.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
chore: add shifts 12/14 - 12/24
</commit_message>
<xml_diff>
--- a/income_sheet.xlsx
+++ b/income_sheet.xlsx
@@ -1191,7 +1191,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E220"/>
+  <dimension ref="A1:E227"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -5164,6 +5164,132 @@
         <v>252.5</v>
       </c>
     </row>
+    <row r="221" ht="13.55" customHeight="1">
+      <c r="A221" s="3">
+        <v>44911</v>
+      </c>
+      <c r="B221" s="4">
+        <v>260</v>
+      </c>
+      <c r="C221" s="4">
+        <v>8.5</v>
+      </c>
+      <c r="D221" s="4">
+        <v>15</v>
+      </c>
+      <c r="E221" s="4">
+        <f>B221+(C221*D221)</f>
+        <v>387.5</v>
+      </c>
+    </row>
+    <row r="222" ht="13.55" customHeight="1">
+      <c r="A222" s="3">
+        <v>44912</v>
+      </c>
+      <c r="B222" s="4">
+        <v>200</v>
+      </c>
+      <c r="C222" s="4">
+        <v>6.5</v>
+      </c>
+      <c r="D222" s="4">
+        <v>15</v>
+      </c>
+      <c r="E222" s="4">
+        <f>B222+(C222*D222)</f>
+        <v>297.5</v>
+      </c>
+    </row>
+    <row r="223" ht="13.55" customHeight="1">
+      <c r="A223" s="3">
+        <v>44913</v>
+      </c>
+      <c r="B223" s="4">
+        <v>613</v>
+      </c>
+      <c r="C223" s="4">
+        <v>12.5</v>
+      </c>
+      <c r="D223" s="4">
+        <v>15</v>
+      </c>
+      <c r="E223" s="4">
+        <f>B223+(C223*D223)</f>
+        <v>800.5</v>
+      </c>
+    </row>
+    <row r="224" ht="13.55" customHeight="1">
+      <c r="A224" s="3">
+        <v>44915</v>
+      </c>
+      <c r="B224" s="4">
+        <v>105</v>
+      </c>
+      <c r="C224" s="4">
+        <v>7</v>
+      </c>
+      <c r="D224" s="4">
+        <v>15</v>
+      </c>
+      <c r="E224" s="4">
+        <f>B224+(C224*D224)</f>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="225" ht="13.55" customHeight="1">
+      <c r="A225" s="3">
+        <v>44916</v>
+      </c>
+      <c r="B225" s="4">
+        <v>230</v>
+      </c>
+      <c r="C225" s="4">
+        <v>7</v>
+      </c>
+      <c r="D225" s="4">
+        <v>15</v>
+      </c>
+      <c r="E225" s="4">
+        <f>B225+(C225*D225)</f>
+        <v>335</v>
+      </c>
+    </row>
+    <row r="226" ht="13.55" customHeight="1">
+      <c r="A226" s="3">
+        <v>44918</v>
+      </c>
+      <c r="B226" s="4">
+        <v>235</v>
+      </c>
+      <c r="C226" s="4">
+        <v>8</v>
+      </c>
+      <c r="D226" s="4">
+        <v>15</v>
+      </c>
+      <c r="E226" s="4">
+        <f>B226+(C226*D226)</f>
+        <v>355</v>
+      </c>
+    </row>
+    <row r="227" ht="13.55" customHeight="1">
+      <c r="A227" s="3">
+        <v>44919</v>
+      </c>
+      <c r="B227" s="4">
+        <v>125</v>
+      </c>
+      <c r="C227" s="4">
+        <v>3</v>
+      </c>
+      <c r="D227" s="4">
+        <v>15</v>
+      </c>
+      <c r="E227" s="4">
+        <f>B227+(C227*D227)</f>
+        <v>170</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>